<commit_message>
Added Seasonallly Adjusted code and text
</commit_message>
<xml_diff>
--- a/LaborData.xlsx
+++ b/LaborData.xlsx
@@ -12,11 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="75">
   <si>
     <t>Series ID</t>
   </si>
   <si>
+    <t>Seasonally Adjusted Code</t>
+  </si>
+  <si>
+    <t>Seasonally Adjusted Text</t>
+  </si>
+  <si>
     <t>State Code</t>
   </si>
   <si>
@@ -57,6 +63,12 @@
   </si>
   <si>
     <t>SMU11000000500000011</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Not Seasonally Adjusted</t>
   </si>
   <si>
     <t>11</t>
@@ -269,7 +281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -318,87 +330,99 @@
       <c r="N1" t="s" s="0">
         <v>13</v>
       </c>
+      <c r="O1" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s" s="0">
         <v>26</v>
@@ -406,1149 +430,1311 @@
       <c r="N3" t="s" s="0">
         <v>27</v>
       </c>
+      <c r="O3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>31</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s" s="0">
         <v>32</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M7" t="s" s="0">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M8" t="s" s="0">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M11" t="s" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="N11" t="s" s="0">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="P11" t="s" s="0">
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L12" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>46</v>
+        <v>32</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>50</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J13" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L13" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M13" t="s" s="0">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="N13" t="s" s="0">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="P13" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J14" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K14" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L14" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="N14" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="O14" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="M14" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="N14" t="s" s="0">
-        <v>49</v>
+      <c r="P14" t="s" s="0">
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J15" t="s" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K15" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L15" t="s" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M15" t="s" s="0">
         <v>26</v>
       </c>
       <c r="N15" t="s" s="0">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="O15" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="P15" t="s" s="0">
+        <v>54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J16" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L16" t="s" s="0">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s" s="0">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="N16" t="s" s="0">
-        <v>59</v>
+        <v>27</v>
+      </c>
+      <c r="O16" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="P16" t="s" s="0">
+        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J17" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L17" t="s" s="0">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="M17" t="s" s="0">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s" s="0">
-        <v>60</v>
+        <v>27</v>
+      </c>
+      <c r="O17" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="P17" t="s" s="0">
+        <v>64</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K18" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L18" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M18" t="s" s="0">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="O18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P18" t="s" s="0">
+        <v>65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J19" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L19" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M19" t="s" s="0">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="N19" t="s" s="0">
-        <v>62</v>
+        <v>32</v>
+      </c>
+      <c r="O19" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="P19" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H20" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J20" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L20" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="N20" t="s" s="0">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="O20" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="P20" t="s" s="0">
+        <v>67</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H21" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J21" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K21" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L21" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M21" t="s" s="0">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="N21" t="s" s="0">
-        <v>64</v>
+        <v>32</v>
+      </c>
+      <c r="O21" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="P21" t="s" s="0">
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J22" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K22" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L22" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M22" t="s" s="0">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>64</v>
+        <v>32</v>
+      </c>
+      <c r="O22" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="P22" t="s" s="0">
+        <v>68</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H23" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J23" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K23" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L23" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M23" t="s" s="0">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="N23" t="s" s="0">
-        <v>65</v>
+        <v>32</v>
+      </c>
+      <c r="O23" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="P23" t="s" s="0">
+        <v>69</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H24" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J24" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K24" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M24" t="s" s="0">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="N24" t="s" s="0">
-        <v>66</v>
+        <v>32</v>
+      </c>
+      <c r="O24" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="P24" t="s" s="0">
+        <v>70</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H25" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J25" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K25" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L25" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M25" t="s" s="0">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="N25" t="s" s="0">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="O25" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="P25" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H26" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J26" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K26" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L26" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M26" t="s" s="0">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>68</v>
+        <v>32</v>
+      </c>
+      <c r="O26" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="P26" t="s" s="0">
+        <v>72</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="I27" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="J27" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="K27" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="L27" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="M27" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="N27" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="O27" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B27" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="C27" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E27" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="F27" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="G27" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="H27" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="I27" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="J27" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="K27" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="L27" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="M27" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="N27" t="s" s="0">
-        <v>67</v>
+      <c r="P27" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G28" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H28" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J28" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K28" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L28" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="M28" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="N28" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="O28" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="M28" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="N28" t="s" s="0">
-        <v>69</v>
+      <c r="P28" t="s" s="0">
+        <v>73</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s" s="0">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G29" t="s" s="0">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H29" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J29" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K29" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L29" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="M29" t="s" s="0">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="N29" t="s" s="0">
-        <v>70</v>
+        <v>32</v>
+      </c>
+      <c r="O29" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="P29" t="s" s="0">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>